<commit_message>
Fixes to ASHRAE34 information
Signed-off-by: Ian Bell <ian.h.bell@gmail.com>
</commit_message>
<xml_diff>
--- a/Vault/ASHRAE34.xlsx
+++ b/Vault/ASHRAE34.xlsx
@@ -8,18 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="90">
   <si>
     <t>trichlorofluoromethane</t>
   </si>
@@ -153,6 +152,9 @@
     <t>E170</t>
   </si>
   <si>
+    <t>Propane</t>
+  </si>
+  <si>
     <t>octafluoropropane</t>
   </si>
   <si>
@@ -204,15 +206,6 @@
     <t>oxygen</t>
   </si>
   <si>
-    <t>ethyl</t>
-  </si>
-  <si>
-    <t>methyl</t>
-  </si>
-  <si>
-    <t>(Reserved</t>
-  </si>
-  <si>
     <t>hydrogen</t>
   </si>
   <si>
@@ -268,6 +261,33 @@
   </si>
   <si>
     <t>CAS #</t>
+  </si>
+  <si>
+    <t>ETHYLENE</t>
+  </si>
+  <si>
+    <t>PROPYLEN</t>
+  </si>
+  <si>
+    <t>R404A</t>
+  </si>
+  <si>
+    <t>R507A</t>
+  </si>
+  <si>
+    <t>R410A</t>
+  </si>
+  <si>
+    <t>R407C</t>
+  </si>
+  <si>
+    <t>PROPANE</t>
+  </si>
+  <si>
+    <t>Ethylene</t>
+  </si>
+  <si>
+    <t>Propylene</t>
   </si>
 </sst>
 </file>
@@ -627,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,13 +677,13 @@
         <v>26</v>
       </c>
       <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s">
         <v>80</v>
-      </c>
-      <c r="F2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1307,7 +1327,7 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C31">
         <v>1000</v>
@@ -1334,7 +1354,7 @@
         <v>218</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C32">
         <v>1000</v>
@@ -1358,10 +1378,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C33">
         <v>1000</v>
@@ -1385,10 +1405,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C34">
         <v>1000</v>
@@ -1412,10 +1432,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C35">
         <v>300</v>
@@ -1442,7 +1462,7 @@
         <v>290</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C36">
         <v>1000</v>
@@ -1466,10 +1486,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C37">
         <v>1000</v>
@@ -1496,7 +1516,7 @@
         <v>600</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C38">
         <v>1000</v>
@@ -1511,10 +1531,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C39">
         <v>1000</v>
@@ -1541,7 +1561,7 @@
         <v>601</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C40">
         <v>600</v>
@@ -1553,10 +1573,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C41">
         <v>600</v>
@@ -1583,7 +1603,7 @@
         <v>610</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C42">
         <v>400</v>
@@ -1598,7 +1618,7 @@
         <v>611</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C43">
         <v>100</v>
@@ -1613,10 +1633,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>620</v>
+        <v>630</v>
       </c>
       <c r="B44" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="I44" t="str">
         <f>[1]!CAS_code("R"&amp;A44)</f>
@@ -1625,10 +1645,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I45" t="str">
         <f>[1]!CAS_code("R"&amp;A45)</f>
@@ -1637,194 +1657,286 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>631</v>
+        <v>702</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>62</v>
+      </c>
+      <c r="D46" t="s">
+        <v>22</v>
       </c>
       <c r="I46" t="str">
         <f>[1]!CAS_code("R"&amp;A46)</f>
-        <v>Fluid name invalid</v>
+        <v>1333-74-0</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D47" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="I47" t="str">
-        <f>[1]!CAS_code("R"&amp;A47)</f>
-        <v>1333-74-0</v>
+        <f>[1]!CAS_code("Helium")</f>
+        <v>7440-59-7</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>704</v>
+        <v>717</v>
       </c>
       <c r="B48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D48" t="s">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="E48">
+        <v>320</v>
+      </c>
+      <c r="F48">
+        <v>0.22</v>
+      </c>
+      <c r="G48">
+        <v>1.4E-2</v>
       </c>
       <c r="I48" t="str">
-        <f>[1]!CAS_code("Helium")</f>
-        <v>7440-59-7</v>
+        <f>[1]!CAS_code("R"&amp;A48)</f>
+        <v>7664-41-7</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D49" t="s">
-        <v>15</v>
-      </c>
-      <c r="E49">
-        <v>320</v>
-      </c>
-      <c r="F49">
-        <v>0.22</v>
-      </c>
-      <c r="G49">
-        <v>1.4E-2</v>
+        <v>2</v>
       </c>
       <c r="I49" t="str">
-        <f>[1]!CAS_code("R"&amp;A49)</f>
-        <v>7664-41-7</v>
+        <f>[1]!CAS_code(B49)</f>
+        <v>7732-18-5</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="B50" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D50" t="s">
         <v>2</v>
       </c>
       <c r="I50" t="str">
         <f>[1]!CAS_code(B50)</f>
-        <v>7732-18-5</v>
+        <v>7440-01-9</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D51" t="s">
         <v>2</v>
       </c>
       <c r="I51" t="str">
         <f>[1]!CAS_code(B51)</f>
-        <v>7440-01-9</v>
+        <v>7727-37-9</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>728</v>
+        <v>732</v>
       </c>
       <c r="B52" t="s">
-        <v>69</v>
-      </c>
-      <c r="D52" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="I52" t="str">
         <f>[1]!CAS_code(B52)</f>
-        <v>7727-37-9</v>
+        <v>7782-44-7</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>732</v>
+        <v>740</v>
       </c>
       <c r="B53" t="s">
-        <v>60</v>
+        <v>68</v>
+      </c>
+      <c r="D53" t="s">
+        <v>2</v>
       </c>
       <c r="I53" t="str">
-        <f>[1]!CAS_code(B53)</f>
-        <v>7782-44-7</v>
+        <f>[1]!CAS_code("Argon")</f>
+        <v>7440-37-1</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>740</v>
+        <v>744</v>
       </c>
       <c r="B54" t="s">
-        <v>70</v>
+        <v>73</v>
+      </c>
+      <c r="C54">
+        <v>5000</v>
       </c>
       <c r="D54" t="s">
         <v>2</v>
       </c>
+      <c r="E54" s="1">
+        <v>40000</v>
+      </c>
+      <c r="F54">
+        <v>72</v>
+      </c>
+      <c r="G54">
+        <v>4.5</v>
+      </c>
       <c r="I54" t="str">
-        <f>[1]!CAS_code("Argon")</f>
-        <v>7440-37-1</v>
+        <f>[1]!CAS_code("R"&amp;A54)</f>
+        <v>124-38-9</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>744</v>
+      <c r="A55" t="s">
+        <v>69</v>
       </c>
       <c r="B55" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55">
-        <v>5000</v>
-      </c>
-      <c r="D55" t="s">
-        <v>2</v>
-      </c>
-      <c r="E55" s="1">
-        <v>40000</v>
-      </c>
-      <c r="F55">
-        <v>72</v>
-      </c>
-      <c r="G55">
-        <v>4.5</v>
+        <v>74</v>
       </c>
       <c r="I55" t="str">
-        <f>[1]!CAS_code("R"&amp;A55)</f>
-        <v>124-38-9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>71</v>
-      </c>
-      <c r="B56" t="s">
-        <v>76</v>
-      </c>
-      <c r="I56" t="str">
         <f>[1]!CAS_code("NitrousOxide")</f>
         <v>10024-97-2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>764</v>
       </c>
-      <c r="B57" t="s">
-        <v>77</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="B56" t="s">
+        <v>75</v>
+      </c>
+      <c r="D56" t="s">
         <v>11</v>
       </c>
-      <c r="I57" t="str">
+      <c r="I56" t="str">
         <f>[1]!CAS_code("SulfurDioxide")</f>
         <v>7446-09-5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>81</v>
+      </c>
+      <c r="B57" t="s">
+        <v>88</v>
+      </c>
+      <c r="D57" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57" t="str">
+        <f>[1]!CAS_code(B57)</f>
+        <v>74-85-1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" t="s">
+        <v>22</v>
+      </c>
+      <c r="I58" t="str">
+        <f>[1]!CAS_code(B58)</f>
+        <v>115-07-1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>83</v>
+      </c>
+      <c r="B59" t="s">
+        <v>83</v>
+      </c>
+      <c r="D59" t="s">
+        <v>2</v>
+      </c>
+      <c r="I59" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" t="s">
+        <v>84</v>
+      </c>
+      <c r="D60" t="s">
+        <v>2</v>
+      </c>
+      <c r="I60" t="str">
+        <f>B60</f>
+        <v>R507A</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" t="s">
+        <v>85</v>
+      </c>
+      <c r="D61" t="s">
+        <v>2</v>
+      </c>
+      <c r="I61" t="str">
+        <f t="shared" ref="I61:I62" si="0">B61</f>
+        <v>R410A</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" t="s">
+        <v>86</v>
+      </c>
+      <c r="D62" t="s">
+        <v>2</v>
+      </c>
+      <c r="I62" t="str">
+        <f t="shared" si="0"/>
+        <v>R407C</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>87</v>
+      </c>
+      <c r="B63" t="s">
+        <v>44</v>
+      </c>
+      <c r="D63" t="s">
+        <v>22</v>
+      </c>
+      <c r="I63" t="str">
+        <f>[1]!CAS_code(B63)</f>
+        <v>74-98-6</v>
       </c>
     </row>
   </sheetData>
@@ -1833,441 +1945,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="A1:G27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="36.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1">
-        <v>1000</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1">
-        <v>8500</v>
-      </c>
-      <c r="F1">
-        <v>16</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>218</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2">
-        <v>1000</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1">
-        <v>90000</v>
-      </c>
-      <c r="F2">
-        <v>690</v>
-      </c>
-      <c r="G2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3">
-        <v>1000</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>84000</v>
-      </c>
-      <c r="F3">
-        <v>580</v>
-      </c>
-      <c r="G3">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4">
-        <v>1000</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1">
-        <v>55000</v>
-      </c>
-      <c r="F4">
-        <v>340</v>
-      </c>
-      <c r="G4">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5">
-        <v>300</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1">
-        <v>34000</v>
-      </c>
-      <c r="F5">
-        <v>190</v>
-      </c>
-      <c r="G5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>290</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6">
-        <v>1000</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6">
-        <v>5300</v>
-      </c>
-      <c r="F6">
-        <v>9.5</v>
-      </c>
-      <c r="G6">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7">
-        <v>1000</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1">
-        <v>69000</v>
-      </c>
-      <c r="F7">
-        <v>570</v>
-      </c>
-      <c r="G7">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>600</v>
-      </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9">
-        <v>1000</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9">
-        <v>4000</v>
-      </c>
-      <c r="F9">
-        <v>9.6</v>
-      </c>
-      <c r="G9">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>601</v>
-      </c>
-      <c r="B10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11">
-        <v>600</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11">
-        <v>1000</v>
-      </c>
-      <c r="F11">
-        <v>2.9</v>
-      </c>
-      <c r="G11">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>610</v>
-      </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>611</v>
-      </c>
-      <c r="B13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13">
-        <v>100</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>620</v>
-      </c>
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>630</v>
-      </c>
-      <c r="B15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>631</v>
-      </c>
-      <c r="B16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>702</v>
-      </c>
-      <c r="B17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>704</v>
-      </c>
-      <c r="B18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>717</v>
-      </c>
-      <c r="B19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19">
-        <v>320</v>
-      </c>
-      <c r="F19">
-        <v>0.22</v>
-      </c>
-      <c r="G19">
-        <v>1.4E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>718</v>
-      </c>
-      <c r="B20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>720</v>
-      </c>
-      <c r="B21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>728</v>
-      </c>
-      <c r="B22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>732</v>
-      </c>
-      <c r="B23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>740</v>
-      </c>
-      <c r="B24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>744</v>
-      </c>
-      <c r="B25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25">
-        <v>5000</v>
-      </c>
-      <c r="D25" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" s="1">
-        <v>40000</v>
-      </c>
-      <c r="F25">
-        <v>72</v>
-      </c>
-      <c r="G25">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>764</v>
-      </c>
-      <c r="B27" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>